<commit_message>
variable definition revision, now using external config.yaml file. readme changed accordingly
</commit_message>
<xml_diff>
--- a/example_outcome/findings-semgrep-1.17.1.xlsx
+++ b/example_outcome/findings-semgrep-1.17.1.xlsx
@@ -191,7 +191,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -214,6 +214,13 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -223,7 +230,7 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
@@ -571,7 +578,7 @@
     <col min="26" max="26" style="5" width="6.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -609,7 +616,7 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -647,7 +654,7 @@
       <c r="Y2" s="3"/>
       <c r="Z2" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
@@ -685,7 +692,7 @@
       <c r="Y3" s="4"/>
       <c r="Z3" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -723,7 +730,7 @@
       <c r="Y4" s="3"/>
       <c r="Z4" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
@@ -761,7 +768,7 @@
       <c r="Y5" s="4"/>
       <c r="Z5" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
@@ -799,7 +806,7 @@
       <c r="Y6" s="3"/>
       <c r="Z6" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
@@ -837,7 +844,7 @@
       <c r="Y7" s="4"/>
       <c r="Z7" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
@@ -875,7 +882,7 @@
       <c r="Y8" s="3"/>
       <c r="Z8" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="4" t="s">
         <v>25</v>
       </c>
@@ -913,7 +920,7 @@
       <c r="Y9" s="4"/>
       <c r="Z9" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="3" t="s">
         <v>25</v>
       </c>
@@ -951,7 +958,7 @@
       <c r="Y10" s="3"/>
       <c r="Z10" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="4" t="s">
         <v>25</v>
       </c>
@@ -989,7 +996,7 @@
       <c r="Y11" s="4"/>
       <c r="Z11" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="3" t="s">
         <v>25</v>
       </c>
@@ -1027,7 +1034,7 @@
       <c r="Y12" s="3"/>
       <c r="Z12" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="4" t="s">
         <v>25</v>
       </c>
@@ -1065,7 +1072,7 @@
       <c r="Y13" s="4"/>
       <c r="Z13" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="3" t="s">
         <v>25</v>
       </c>
@@ -1103,7 +1110,7 @@
       <c r="Y14" s="3"/>
       <c r="Z14" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="4" t="s">
         <v>25</v>
       </c>
@@ -1141,7 +1148,7 @@
       <c r="Y15" s="4"/>
       <c r="Z15" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="3" t="s">
         <v>25</v>
       </c>
@@ -1179,7 +1186,7 @@
       <c r="Y16" s="3"/>
       <c r="Z16" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="4" t="s">
         <v>25</v>
       </c>
@@ -1217,7 +1224,7 @@
       <c r="Y17" s="4"/>
       <c r="Z17" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="3" t="s">
         <v>25</v>
       </c>
@@ -1255,7 +1262,7 @@
       <c r="Y18" s="3"/>
       <c r="Z18" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="4" t="s">
         <v>25</v>
       </c>
@@ -1293,7 +1300,7 @@
       <c r="Y19" s="4"/>
       <c r="Z19" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="3" t="s">
         <v>25</v>
       </c>
@@ -1331,7 +1338,7 @@
       <c r="Y20" s="3"/>
       <c r="Z20" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="4" t="s">
         <v>25</v>
       </c>
@@ -1369,7 +1376,7 @@
       <c r="Y21" s="4"/>
       <c r="Z21" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="3" t="s">
         <v>25</v>
       </c>

</xml_diff>